<commit_message>
upload 3d ref organs, metadata
</commit_message>
<xml_diff>
--- a/digital-objects/omap/12-eye-retina-ibex/v1.1/raw/omap-12-eye-retina-ibex.xlsx
+++ b/digital-objects/omap/12-eye-retina-ibex/v1.1/raw/omap-12-eye-retina-ibex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellenmq/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellenmq/Documents/GitHub/hra-kg/digital-objects/omap/12-eye-retina-ibex/v1.1/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D53E47-0A2E-4A4B-9AC5-AC1CC567F54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC50EBA-E78A-F044-B1F3-95462AA41EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="760" windowWidth="34560" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5840" yWindow="6540" windowWidth="34560" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="omap-12-eye-retina-ibex" sheetId="1" r:id="rId1"/>
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:AR1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>